<commit_message>
working code, using test.xlsx to test
</commit_message>
<xml_diff>
--- a/weekies_ver_03/test.xlsx
+++ b/weekies_ver_03/test.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\weekies_ver_03\weekies_ver_03\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C2C126F1-F623-44E0-9E1F-3D0C85425D9B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16100" xWindow="8610" yWindow="20"/>
   </bookViews>
   <sheets>
-    <sheet name="2018" sheetId="1" r:id="rId1"/>
+    <sheet name="2018" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Count</t>
   </si>
@@ -44,6 +38,9 @@
   </si>
   <si>
     <t>Simon</t>
+  </si>
+  <si>
+    <t>2018-07-19</t>
   </si>
   <si>
     <t>Prada</t>
@@ -118,19 +115,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -146,25 +144,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="一般" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -488,19 +477,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="16.7265625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,12 +503,12 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="n">
         <v>43259</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:4">
+      <c r="A2" t="n">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -524,12 +517,12 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="n">
         <v>43259</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:4">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -538,12 +531,12 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>43252</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:4">
+      <c r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -552,13 +545,13 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="n">
         <v>43253</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3</v>
+    <row r="5" spans="1:4">
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -566,306 +559,306 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1">
-        <v>43254</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>2</v>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="n">
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>43279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>43294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>43176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>43287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>43300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>43272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>43292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>43300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>43161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1">
-        <v>43245</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1">
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>43262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1" t="n">
         <v>43279</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1">
+    <row r="20" spans="1:4">
+      <c r="A20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>43231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>43287</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>43294</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1">
-        <v>43238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1">
-        <v>43287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1">
-        <v>43266</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1">
-        <v>43252</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="1">
+    <row r="25" spans="1:4">
+      <c r="A25" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="1" t="n">
         <v>43272</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1">
-        <v>43133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="1">
-        <v>43140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="1">
-        <v>43161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1">
-        <v>43162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="1">
-        <v>43163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="1">
-        <v>43279</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="1">
-        <v>43231</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="1">
-        <v>43101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" t="n">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="1">
-        <v>43287</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="1">
-        <v>43266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="1">
-        <v>43294</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="1">
-        <v>43272</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
       <c r="C26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="1">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1" t="n">
         <v>43259</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>